<commit_message>
new benchmark with kcptun
</commit_message>
<xml_diff>
--- a/benchmarks/TCPvsDragonite.xlsx
+++ b/benchmarks/TCPvsDragonite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Network Environment</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,6 +59,10 @@
   </si>
   <si>
     <t>TCP-BBR Performance (MBytes/sec)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kcptun -fast Performance (MBytes/sec)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -352,8 +356,108 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100Mbps 25ms'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kcptun -fast Performance (MBytes/sec)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100Mbps 25ms'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.01% loss</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1% loss</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1% loss</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10% loss</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20% loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100Mbps 25ms'!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-43A9-4489-9CAF-1057B252E1FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'100Mbps 25ms'!$D$1</c:f>
@@ -1135,9 +1239,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>685801</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1462,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08920676-1FF9-4E90-8A5A-7C365603130C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1474,9 +1578,10 @@
     <col min="2" max="2" width="33.75" customWidth="1"/>
     <col min="3" max="3" width="32.125" customWidth="1"/>
     <col min="4" max="4" width="34.375" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,8 +1594,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1503,8 +1611,11 @@
       <c r="D2">
         <v>11.7</v>
       </c>
+      <c r="E2">
+        <v>9.1199999999999992</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1517,8 +1628,11 @@
       <c r="D3">
         <v>11.5</v>
       </c>
+      <c r="E3">
+        <v>8.25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1531,8 +1645,11 @@
       <c r="D4">
         <v>11.3</v>
       </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1545,8 +1662,11 @@
       <c r="D5">
         <v>7.73</v>
       </c>
+      <c r="E5">
+        <v>6.75</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1558,6 +1678,9 @@
       </c>
       <c r="D6">
         <v>5.17</v>
+      </c>
+      <c r="E6">
+        <v>4.0999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add benchmark image to README
</commit_message>
<xml_diff>
--- a/benchmarks/TCPvsDragonite.xlsx
+++ b/benchmarks/TCPvsDragonite.xlsx
@@ -162,7 +162,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>TCP vs Dragonite (100Mbps 25ms)</a:t>
+              <a:t>TCP vs KCP vs Dragonite (100Mbps 25ms)</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>